<commit_message>
Consolidate manufacturing industry ISIC data in non IO files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoDSCbRIC/Shr of Dist Solar Costs by Rcpnt ISIC Code.xlsx
+++ b/InputData/bldgs/SoDSCbRIC/Shr of Dist Solar Costs by Rcpnt ISIC Code.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\bldgs\SoDSCbRIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-mexico\InputData\bldgs\SoDSCbRIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE39E34D-69A6-4F3D-B443-E81143DC1E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="105" windowWidth="25665" windowHeight="16830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="105" windowWidth="25665" windowHeight="16830"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="SoDSCbRIC" sheetId="2" r:id="rId3"/>
+    <sheet name="Pre ISIC Consolidation" sheetId="4" r:id="rId3"/>
+    <sheet name="SoDSCbRIC" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="128">
   <si>
     <t>https://www.nrel.gov/docs/fy19osti/72399.pdf</t>
   </si>
@@ -407,12 +407,24 @@
   </si>
   <si>
     <t>Water and waste</t>
+  </si>
+  <si>
+    <t>EU ISIC Consolidation</t>
+  </si>
+  <si>
+    <t>Default EPS ISIC Groupings</t>
+  </si>
+  <si>
+    <t>Distributed Solar</t>
+  </si>
+  <si>
+    <t>Mexico ISIC Groupings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +482,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -485,7 +503,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -503,6 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -784,22 +803,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -807,49 +826,49 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -857,22 +876,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="66.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.73046875" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" customWidth="1"/>
+    <col min="5" max="5" width="11.265625" customWidth="1"/>
+    <col min="7" max="7" width="11.86328125" customWidth="1"/>
+    <col min="8" max="8" width="66.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -887,7 +906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
@@ -910,7 +929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -935,7 +954,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -960,7 +979,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -985,7 +1004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1010,7 +1029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1056,7 +1075,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1175,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1200,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G14" t="s">
         <v>65</v>
       </c>
@@ -1189,7 +1208,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1204,7 +1223,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1246,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1277,7 +1296,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1302,7 +1321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1348,7 +1367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1373,7 +1392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1398,7 +1417,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1448,7 +1467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1473,7 +1492,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1517,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G28" t="s">
         <v>120</v>
       </c>
@@ -1506,7 +1525,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G29" t="s">
         <v>73</v>
       </c>
@@ -1514,7 +1533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G30" t="s">
         <v>74</v>
       </c>
@@ -1522,7 +1541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G31" t="s">
         <v>75</v>
       </c>
@@ -1530,7 +1549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G32" t="s">
         <v>76</v>
       </c>
@@ -1538,7 +1557,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G33" t="s">
         <v>77</v>
       </c>
@@ -1546,7 +1565,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G34" t="s">
         <v>78</v>
       </c>
@@ -1554,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G35" t="s">
         <v>79</v>
       </c>
@@ -1562,7 +1581,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G36" t="s">
         <v>80</v>
       </c>
@@ -1570,7 +1589,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G37" t="s">
         <v>81</v>
       </c>
@@ -1578,7 +1597,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G38" t="s">
         <v>82</v>
       </c>
@@ -1586,7 +1605,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G39" t="s">
         <v>83</v>
       </c>
@@ -1594,7 +1613,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G40" t="s">
         <v>84</v>
       </c>
@@ -1602,7 +1621,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G41" t="s">
         <v>85</v>
       </c>
@@ -1610,7 +1629,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G42" t="s">
         <v>86</v>
       </c>
@@ -1618,7 +1637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.45">
       <c r="G43" t="s">
         <v>55</v>
       </c>
@@ -1632,20 +1651,1046 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:AQ10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!B2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!C2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!D2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!E2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!F2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!G2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!H2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!I2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!J2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!K2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!L2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!M2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!N2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!O2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!P2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!Q2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!R2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!S2,Data!$D$3:$D$13)</f>
+        <v>5.7183142722857593E-2</v>
+      </c>
+      <c r="T3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!T2,Data!$D$3:$D$13)</f>
+        <v>0.1818110606297979</v>
+      </c>
+      <c r="U3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!U2,Data!$D$3:$D$13)</f>
+        <v>0.18846937176876077</v>
+      </c>
+      <c r="V3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!V2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!W2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!X2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!Y2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!Z2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AA2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AB2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AC2,Data!$D$3:$D$13)</f>
+        <v>0.30988563371455435</v>
+      </c>
+      <c r="AD3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AD2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AE2,Data!$D$3:$D$13)</f>
+        <v>0.12454958483471723</v>
+      </c>
+      <c r="AF3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AF2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AG2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AH2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AI2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AJ2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AK2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AL2,Data!$D$3:$D$13)</f>
+        <v>0.13810120632931225</v>
+      </c>
+      <c r="AM3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AM2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AN2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AO2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AP2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <f>SUMIF(Data!$E$3:$E$13,'Pre ISIC Consolidation'!AQ2,Data!$D$3:$D$13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:AQ4" si="0">C3</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>5.7183142722857593E-2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>0.1818110606297979</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>0.18846937176876077</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="0"/>
+        <v>0.30988563371455435</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="0"/>
+        <v>0.12454958483471723</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="0"/>
+        <v>0.13810120632931225</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!B2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!C2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!D2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!E2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!F2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!G2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!H2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!I2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!J2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!K2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!L2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!M2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!N2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!O2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!P2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!Q2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!R2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!S2,Data!$D$17:$D$27)</f>
+        <v>8.9657692776221209E-2</v>
+      </c>
+      <c r="T5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!T2,Data!$D$17:$D$27)</f>
+        <v>0.26233402363259839</v>
+      </c>
+      <c r="U5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!U2,Data!$D$17:$D$27)</f>
+        <v>0.16944816664636375</v>
+      </c>
+      <c r="V5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!V2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!W2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!X2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!Y2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!Z2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AA2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AB2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AC2,Data!$D$17:$D$27)</f>
+        <v>0.42922402241442315</v>
+      </c>
+      <c r="AD5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AD2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AE2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AF2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AG2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AH2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AI2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AJ2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AK2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AL2,Data!$D$17:$D$27)</f>
+        <v>4.9336094530393476E-2</v>
+      </c>
+      <c r="AM5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AM2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AN2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AO2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AP2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <f>SUMIF(Data!$E$17:$E$27,'Pre ISIC Consolidation'!AQ2,Data!$D$17:$D$27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="11"/>
+      <c r="AQ8" s="11"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL9" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO9" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ9" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z10" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM10" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP10" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ10" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AQ4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B1" s="10" t="s">
         <v>57</v>
       </c>
@@ -1773,522 +2818,522 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!B1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!B$1)</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!C1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!C$1)</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!D1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!D$1)</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!E1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!E$1)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!F1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!F$1)</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!G1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!G$1)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!H1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!H$1)</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!I1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!I$1)</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!J1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!J$1)</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!K1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!K$1)</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!L1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!L$1)</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!M1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!M$1)</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!N1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!N$1)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!O1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!O$1)</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!P1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!P$1)</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Q1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Q$1)</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!R1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!R$1)</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!S1,Data!$D$3:$D$13)</f>
-        <v>5.7183142722857593E-2</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!S$1)</f>
+        <v>0</v>
       </c>
       <c r="T2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!T1,Data!$D$3:$D$13)</f>
-        <v>0.1818110606297979</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!T$1)</f>
+        <v>0</v>
       </c>
       <c r="U2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!U1,Data!$D$3:$D$13)</f>
-        <v>0.18846937176876077</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!U$1)</f>
+        <v>0</v>
       </c>
       <c r="V2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!V1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!V$1)</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!W1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!W$1)</f>
         <v>0</v>
       </c>
       <c r="X2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!X1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!X$1)</f>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Y1,Data!$D$3:$D$13)</f>
-        <v>0</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Y$1)</f>
+        <v>0.42746357512141631</v>
       </c>
       <c r="Z2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!Z1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Z$1)</f>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AA1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AA$1)</f>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AB1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AB$1)</f>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AC1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AC$1)</f>
         <v>0.30988563371455435</v>
       </c>
       <c r="AD2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AD1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AD$1)</f>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AE1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AE$1)</f>
         <v>0.12454958483471723</v>
       </c>
       <c r="AF2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AF1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AF$1)</f>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AG1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AG$1)</f>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AH1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AH$1)</f>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AI1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AI$1)</f>
         <v>0</v>
       </c>
       <c r="AJ2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AJ1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AJ$1)</f>
         <v>0</v>
       </c>
       <c r="AK2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AK1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AK$1)</f>
         <v>0</v>
       </c>
       <c r="AL2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AL1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AL$1)</f>
         <v>0.13810120632931225</v>
       </c>
       <c r="AM2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AM1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AM$1)</f>
         <v>0</v>
       </c>
       <c r="AN2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AN1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AN$1)</f>
         <v>0</v>
       </c>
       <c r="AO2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AO1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AO$1)</f>
         <v>0</v>
       </c>
       <c r="AP2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AP1,Data!$D$3:$D$13)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AP$1)</f>
         <v>0</v>
       </c>
       <c r="AQ2">
-        <f>SUMIF(Data!$E$3:$E$13,SoDSCbRIC!AQ1,Data!$D$3:$D$13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+        <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AQ$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>88</v>
       </c>
       <c r="B3">
-        <f>B2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!B$1)</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:AQ3" si="0">C2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!C$1)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3" si="1">D2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!D$1)</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!E$1)</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!F$1)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!G$1)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!H$1)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!I$1)</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!J$1)</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!K$1)</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!L$1)</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3" si="2">M2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!M$1)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!N$1)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!O$1)</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3" si="3">P2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!P$1)</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Q$1)</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3" si="4">R2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!R$1)</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
-        <v>5.7183142722857593E-2</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!S$1)</f>
+        <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
-        <v>0.1818110606297979</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!T$1)</f>
+        <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
-        <v>0.18846937176876077</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!U$1)</f>
+        <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!V$1)</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!W$1)</f>
         <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!X$1)</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Y$1)</f>
+        <v>0.42746357512141631</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Z$1)</f>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AB3" si="5">AA2</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AA$1)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="5"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AB$1)</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AC$1)</f>
         <v>0.30988563371455435</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AD$1)</f>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AE$1)</f>
         <v>0.12454958483471723</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AF$1)</f>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AG$1)</f>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AH$1)</f>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AI$1)</f>
         <v>0</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AJ$1)</f>
         <v>0</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AK$1)</f>
         <v>0</v>
       </c>
       <c r="AL3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AL$1)</f>
         <v>0.13810120632931225</v>
       </c>
       <c r="AM3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AM$1)</f>
         <v>0</v>
       </c>
       <c r="AN3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AN$1)</f>
         <v>0</v>
       </c>
       <c r="AO3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AO$1)</f>
         <v>0</v>
       </c>
       <c r="AP3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AP$1)</f>
         <v>0</v>
       </c>
       <c r="AQ3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+        <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AQ$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>89</v>
       </c>
       <c r="B4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!B1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!B$1)</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!C1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!C$1)</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!D1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!D$1)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!E1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!E$1)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!F1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!F$1)</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!G1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!G$1)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!H1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!H$1)</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!I1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!I$1)</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!J1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!J$1)</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!K1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!K$1)</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!L1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!L$1)</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!M1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!M$1)</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!N1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!N$1)</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!O1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!O$1)</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!P1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!P$1)</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Q1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Q$1)</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!R1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!R$1)</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!S1,Data!$D$17:$D$27)</f>
-        <v>8.9657692776221209E-2</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!S$1)</f>
+        <v>0</v>
       </c>
       <c r="T4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!T1,Data!$D$17:$D$27)</f>
-        <v>0.26233402363259839</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!T$1)</f>
+        <v>0</v>
       </c>
       <c r="U4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!U1,Data!$D$17:$D$27)</f>
-        <v>0.16944816664636375</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!U$1)</f>
+        <v>0</v>
       </c>
       <c r="V4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!V1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!V$1)</f>
         <v>0</v>
       </c>
       <c r="W4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!W1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!W$1)</f>
         <v>0</v>
       </c>
       <c r="X4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!X1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!X$1)</f>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Y1,Data!$D$17:$D$27)</f>
-        <v>0</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Y$1)</f>
+        <v>0.52143988305518341</v>
       </c>
       <c r="Z4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!Z1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!Z$1)</f>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AA1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AA$1)</f>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AB1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AB$1)</f>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AC1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AC$1)</f>
         <v>0.42922402241442315</v>
       </c>
       <c r="AD4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AD1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AD$1)</f>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AE1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AE$1)</f>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AF1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AF$1)</f>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AG1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AG$1)</f>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AH1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AH$1)</f>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AI1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AI$1)</f>
         <v>0</v>
       </c>
       <c r="AJ4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AJ1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AJ$1)</f>
         <v>0</v>
       </c>
       <c r="AK4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AK1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AK$1)</f>
         <v>0</v>
       </c>
       <c r="AL4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AL1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AL$1)</f>
         <v>4.9336094530393476E-2</v>
       </c>
       <c r="AM4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AM1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AM$1)</f>
         <v>0</v>
       </c>
       <c r="AN4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AN1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AN$1)</f>
         <v>0</v>
       </c>
       <c r="AO4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AO1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AO$1)</f>
         <v>0</v>
       </c>
       <c r="AP4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AP1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AP$1)</f>
         <v>0</v>
       </c>
       <c r="AQ4">
-        <f>SUMIF(Data!$E$17:$E$27,SoDSCbRIC!AQ1,Data!$D$17:$D$27)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$10:$AQ$10,SoDSCbRIC!AQ$1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>